<commit_message>
Uploading all files to git - including PI files
</commit_message>
<xml_diff>
--- a/Validation Documentation/Reference 3.2.1.4.xlsx
+++ b/Validation Documentation/Reference 3.2.1.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/00404ad8203d4b15/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojok\Desktop\2022 - Spring\ECEN 404\Validation Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_F25DC773A252ABDACC10484481D873EA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD0BBAEC-3B2E-4734-9C4E-0C88E838E2E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A075B0-EDFF-427C-8F66-496DE27F4E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27675" yWindow="1185" windowWidth="21600" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Rating:</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>This test was given to a potential user of this project. The user interacted with the GUI after 3 minutes of instruction. The user then rated each category of the GUI based off of their experience.</t>
+  </si>
+  <si>
+    <t>Rating (1-10):</t>
   </si>
 </sst>
 </file>
@@ -109,12 +112,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,8 +138,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,6 +165,30 @@
     <tableColumn id="1" xr3:uid="{237D93B4-BADC-421F-BBD4-D481BFE32248}" name="Category:"/>
     <tableColumn id="2" xr3:uid="{634F3A46-3B34-4BD9-BF63-E15E2CCBEB18}" name="Rating:"/>
     <tableColumn id="3" xr3:uid="{87D9F210-1C7F-4ECB-834B-00A14646ECB4}" name="Comments:"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{39658D5B-B7DD-4318-B87A-B18C655573A4}" name="Table13" displayName="Table13" ref="A19:C25" totalsRowShown="0">
+  <autoFilter ref="A19:C25" xr:uid="{39658D5B-B7DD-4318-B87A-B18C655573A4}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9EBC0BA6-76C4-459B-B40E-DDC8EBD6A5AB}" name="Category:"/>
+    <tableColumn id="2" xr3:uid="{7F4911DC-FBBC-45CD-A7F4-1398B60AD5B1}" name="Rating (1-10):"/>
+    <tableColumn id="3" xr3:uid="{DE8775FB-FF54-442F-AEEE-F38D24E08C54}" name="Comments:"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5E8A926A-86F3-42DD-970F-D198B056CDCC}" name="Table134" displayName="Table134" ref="A27:C33" totalsRowShown="0">
+  <autoFilter ref="A27:C33" xr:uid="{5E8A926A-86F3-42DD-970F-D198B056CDCC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0B4A2AD5-FFB8-4C00-87D0-85C068B51C38}" name="Category:"/>
+    <tableColumn id="2" xr3:uid="{E57B9A35-8708-4D32-ABB0-76401943526F}" name="Rating (1-10):"/>
+    <tableColumn id="3" xr3:uid="{9772FD83-7A9A-4B89-917A-39790CF9CA9F}" name="Comments:"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -423,21 +457,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" customWidth="1"/>
     <col min="3" max="3" width="131" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -445,18 +479,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -467,7 +501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -478,7 +512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -489,7 +523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -500,7 +534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -511,7 +545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -520,7 +554,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -528,25 +562,134 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <f>SUM(B28:B31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>